<commit_message>
Replace xlrd with xsl to improve the speed of reading Excel
</commit_message>
<xml_diff>
--- a/test/测试文件1.xlsx
+++ b/test/测试文件1.xlsx
@@ -154,9 +154,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -167,6 +167,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -175,15 +217,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +243,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -198,39 +258,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -242,6 +280,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -250,62 +296,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,31 +320,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,151 +470,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,17 +514,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,17 +538,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,17 +571,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,11 +597,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,10 +619,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -631,144 +631,141 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1119,21 +1116,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="3" width="12.625"/>
-    <col min="4" max="4" width="16.6333333333333" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="24.875" customWidth="1"/>
-    <col min="9" max="9" width="11.3416666666667" customWidth="1"/>
-    <col min="10" max="10" width="38.8416666666667" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
+    <col min="10" max="10" width="38.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1174,11 +1171,11 @@
       </c>
       <c r="B2">
         <f ca="1" t="shared" ref="B2:B7" si="0">RANDBETWEEN(10,100)</f>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <f ca="1" t="shared" ref="C2:C7" si="1">RAND()</f>
-        <v>0.447456958865866</v>
+        <v>0.298153882839807</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -1205,11 +1202,11 @@
       </c>
       <c r="B3">
         <f ca="1" t="shared" si="0"/>
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <f ca="1" t="shared" si="1"/>
-        <v>0.128566368625415</v>
+        <v>0.325982714273084</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -1239,11 +1236,11 @@
       </c>
       <c r="B4">
         <f ca="1" t="shared" si="0"/>
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <f ca="1" t="shared" si="1"/>
-        <v>0.84116860375399</v>
+        <v>0.05056269044337</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
@@ -1270,11 +1267,11 @@
       </c>
       <c r="B5">
         <f ca="1" t="shared" si="0"/>
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <f ca="1" t="shared" si="1"/>
-        <v>0.672343821831998</v>
+        <v>0.858495728062751</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>25</v>
@@ -1301,11 +1298,11 @@
       </c>
       <c r="B6">
         <f ca="1" t="shared" si="0"/>
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <f ca="1" t="shared" si="1"/>
-        <v>0.539856431001519</v>
+        <v>0.0579463965141798</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>30</v>
@@ -1335,11 +1332,11 @@
       </c>
       <c r="B7">
         <f ca="1" t="shared" si="0"/>
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <f ca="1" t="shared" si="1"/>
-        <v>0.643691913535744</v>
+        <v>0.364418853042751</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>35</v>
@@ -1364,7 +1361,6 @@
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E8"/>
       <c r="H8" t="s">
         <v>40</v>
       </c>
@@ -1376,21 +1372,12 @@
       <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9"/>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="4:5">
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="4:5">
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>